<commit_message>
Função do histograma implementada em assembly + copia das funções em C e em assembly para a ram + usando funções da ram
</commit_message>
<xml_diff>
--- a/Lab2/Histograms.xlsx
+++ b/Lab2/Histograms.xlsx
@@ -4,12 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="36" windowWidth="22980" windowHeight="9552"/>
   </bookViews>
   <sheets>
-    <sheet name="img1" sheetId="1" r:id="rId1"/>
-    <sheet name="img2" sheetId="2" r:id="rId2"/>
-    <sheet name="Plan3" sheetId="3" r:id="rId3"/>
+    <sheet name="img0" sheetId="1" r:id="rId1"/>
+    <sheet name="img1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
@@ -89,6 +88,21 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>image0 Histogram</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
     </c:title>
@@ -103,12 +117,12 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>image1 Histogram</c:v>
+            <c:v>image0 Histogram</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'img1'!$A$2:$A$257</c:f>
+              <c:f>img0!$A$2:$A$257</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -885,7 +899,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'img1'!$B$2:$B$257</c:f>
+              <c:f>img0!$B$2:$B$257</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -1670,11 +1684,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="69244800"/>
-        <c:axId val="69246336"/>
+        <c:axId val="123784576"/>
+        <c:axId val="123794560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="69244800"/>
+        <c:axId val="123784576"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1684,7 +1698,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69246336"/>
+        <c:crossAx val="123794560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1692,7 +1706,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="69246336"/>
+        <c:axId val="123794560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1703,7 +1717,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="69244800"/>
+        <c:crossAx val="123784576"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1740,8 +1754,26 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>image1 Histogram</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:layout/>
       <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+      </c:spPr>
     </c:title>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
@@ -1754,12 +1786,12 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>image2 Histogram</c:v>
+            <c:v>image1 Histogram</c:v>
           </c:tx>
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:numRef>
-              <c:f>'img2'!$A$2:$A$257</c:f>
+              <c:f>'img1'!$A$2:$A$257</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -2536,7 +2568,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'img2'!$B$2:$B$257</c:f>
+              <c:f>'img1'!$B$2:$B$257</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="256"/>
@@ -3321,11 +3353,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="61257984"/>
-        <c:axId val="83488768"/>
+        <c:axId val="124225024"/>
+        <c:axId val="124226560"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="61257984"/>
+        <c:axId val="124225024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3335,7 +3367,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="83488768"/>
+        <c:crossAx val="124226560"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3343,7 +3375,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="83488768"/>
+        <c:axId val="124226560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3354,7 +3386,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="61257984"/>
+        <c:crossAx val="124225024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3735,8 +3767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B257"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="Q20" sqref="Q20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5807,8 +5839,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T257"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7875,16 +7907,4 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>